<commit_message>
Alterando a documentação do projeto
</commit_message>
<xml_diff>
--- a/Documentação/ListaDeTarefas.xlsx
+++ b/Documentação/ListaDeTarefas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\acheiLink\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC821249-B8DC-45C7-8177-6571202023B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51CF68-D307-4F23-87DF-52BD6267FE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>Id</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>1.4</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Desenvolver api</t>
   </si>
 </sst>
 </file>
@@ -331,7 +337,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -442,19 +448,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -463,14 +463,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,12 +781,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="7" t="s">
         <v>48</v>
       </c>
@@ -1058,13 +1064,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1283,22 +1289,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84120AE-8945-4105-9E02-C5FE2E39E216}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1306,219 +1312,266 @@
       <c r="A1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="11">
         <v>44687</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>44687</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="11">
+        <v>44696</v>
+      </c>
+      <c r="F4" s="11">
+        <v>44696</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="11">
+        <v>44700</v>
+      </c>
+      <c r="F5" s="11">
+        <v>44700</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11">
+        <v>44700</v>
+      </c>
+      <c r="F6" s="11">
+        <v>44700</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11">
+        <v>44700</v>
+      </c>
+      <c r="F7" s="11">
+        <v>44700</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="14" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="B11" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="11" t="s">
+    <row r="13" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="11" t="s">
+    <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>3</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>4</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>5</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>6</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>7</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>8</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+    <row r="18" spans="2:2" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>